<commit_message>
fix bug kwr003 - #118414
</commit_message>
<xml_diff>
--- a/nts.uk/uk.at/at.file/nts.uk.file.at.infra/src/main/resources/report/KWR003_template.xlsx
+++ b/nts.uk/uk.at/at.file/nts.uk.file.at.infra/src/main/resources/report/KWR003_template.xlsx
@@ -293,6 +293,30 @@
     <xf numFmtId="49" fontId="4" fillId="6" borderId="11" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="49" fontId="4" fillId="6" borderId="10" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="6" borderId="11" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="6" borderId="12" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="6" borderId="10" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="8" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="9" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
+    </xf>
     <xf numFmtId="49" fontId="4" fillId="4" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
@@ -304,30 +328,6 @@
     </xf>
     <xf numFmtId="49" fontId="4" fillId="5" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="8" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="9" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="6" borderId="10" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="6" borderId="11" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="6" borderId="12" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="6" borderId="10" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -605,9 +605,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AJ22"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageLayout" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageLayout" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="3.75" defaultRowHeight="9.75"/>
+  <sheetFormatPr defaultColWidth="3.75" defaultRowHeight="13.5" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="1.375" style="2" customWidth="1"/>
     <col min="2" max="3" width="6.75" style="2" customWidth="1"/>
@@ -617,7 +619,7 @@
     <col min="21" max="16384" width="3.75" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" ht="14.25" customHeight="1" thickBot="1">
+    <row r="1" spans="1:36" ht="13.5" customHeight="1" thickBot="1">
       <c r="A1" s="4"/>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
@@ -655,10 +657,10 @@
       <c r="AI1" s="6"/>
       <c r="AJ1" s="6"/>
     </row>
-    <row r="2" spans="1:36" ht="11.25" customHeight="1" thickBot="1">
-      <c r="A2" s="15"/>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
+    <row r="2" spans="1:36" ht="13.5" customHeight="1" thickBot="1">
+      <c r="A2" s="23"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
       <c r="F2" s="7"/>
@@ -690,13 +692,13 @@
       <c r="AF2" s="7"/>
       <c r="AG2" s="7"/>
       <c r="AH2" s="7"/>
-      <c r="AI2" s="16"/>
-      <c r="AJ2" s="16"/>
-    </row>
-    <row r="3" spans="1:36" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A3" s="15"/>
-      <c r="B3" s="15"/>
-      <c r="C3" s="15"/>
+      <c r="AI2" s="24"/>
+      <c r="AJ2" s="24"/>
+    </row>
+    <row r="3" spans="1:36" ht="13.5" customHeight="1" thickBot="1">
+      <c r="A3" s="23"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="23"/>
       <c r="D3" s="8"/>
       <c r="E3" s="8"/>
       <c r="F3" s="8"/>
@@ -728,86 +730,86 @@
       <c r="AF3" s="8"/>
       <c r="AG3" s="8"/>
       <c r="AH3" s="8"/>
-      <c r="AI3" s="16"/>
-      <c r="AJ3" s="16"/>
-    </row>
-    <row r="4" spans="1:36" ht="10.5" thickBot="1">
-      <c r="A4" s="17"/>
-      <c r="B4" s="17"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="17"/>
-      <c r="H4" s="17"/>
-      <c r="I4" s="17"/>
-      <c r="J4" s="17"/>
-      <c r="K4" s="17"/>
-      <c r="L4" s="17"/>
-      <c r="M4" s="17"/>
-      <c r="N4" s="17"/>
-      <c r="O4" s="17"/>
-      <c r="P4" s="17"/>
-      <c r="Q4" s="17"/>
-      <c r="R4" s="17"/>
-      <c r="S4" s="17"/>
-      <c r="T4" s="17"/>
-      <c r="U4" s="17"/>
-      <c r="V4" s="17"/>
-      <c r="W4" s="17"/>
-      <c r="X4" s="17"/>
-      <c r="Y4" s="17"/>
-      <c r="Z4" s="17"/>
-      <c r="AA4" s="17"/>
-      <c r="AB4" s="17"/>
-      <c r="AC4" s="17"/>
-      <c r="AD4" s="17"/>
-      <c r="AE4" s="17"/>
-      <c r="AF4" s="17"/>
-      <c r="AG4" s="17"/>
-      <c r="AH4" s="17"/>
+      <c r="AI3" s="24"/>
+      <c r="AJ3" s="24"/>
+    </row>
+    <row r="4" spans="1:36" ht="13.5" customHeight="1" thickBot="1">
+      <c r="A4" s="25"/>
+      <c r="B4" s="25"/>
+      <c r="C4" s="25"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="25"/>
+      <c r="H4" s="25"/>
+      <c r="I4" s="25"/>
+      <c r="J4" s="25"/>
+      <c r="K4" s="25"/>
+      <c r="L4" s="25"/>
+      <c r="M4" s="25"/>
+      <c r="N4" s="25"/>
+      <c r="O4" s="25"/>
+      <c r="P4" s="25"/>
+      <c r="Q4" s="25"/>
+      <c r="R4" s="25"/>
+      <c r="S4" s="25"/>
+      <c r="T4" s="25"/>
+      <c r="U4" s="25"/>
+      <c r="V4" s="25"/>
+      <c r="W4" s="25"/>
+      <c r="X4" s="25"/>
+      <c r="Y4" s="25"/>
+      <c r="Z4" s="25"/>
+      <c r="AA4" s="25"/>
+      <c r="AB4" s="25"/>
+      <c r="AC4" s="25"/>
+      <c r="AD4" s="25"/>
+      <c r="AE4" s="25"/>
+      <c r="AF4" s="25"/>
+      <c r="AG4" s="25"/>
+      <c r="AH4" s="25"/>
       <c r="AI4" s="9"/>
       <c r="AJ4" s="9"/>
     </row>
-    <row r="5" spans="1:36" ht="10.5" thickBot="1">
-      <c r="A5" s="18"/>
-      <c r="B5" s="18"/>
-      <c r="C5" s="18"/>
-      <c r="D5" s="18"/>
-      <c r="E5" s="18"/>
-      <c r="F5" s="18"/>
-      <c r="G5" s="18"/>
-      <c r="H5" s="18"/>
-      <c r="I5" s="18"/>
-      <c r="J5" s="18"/>
-      <c r="K5" s="18"/>
-      <c r="L5" s="18"/>
-      <c r="M5" s="18"/>
-      <c r="N5" s="18"/>
-      <c r="O5" s="18"/>
-      <c r="P5" s="18"/>
-      <c r="Q5" s="18"/>
-      <c r="R5" s="18"/>
-      <c r="S5" s="18"/>
-      <c r="T5" s="18"/>
-      <c r="U5" s="18"/>
-      <c r="V5" s="18"/>
-      <c r="W5" s="18"/>
-      <c r="X5" s="18"/>
-      <c r="Y5" s="18"/>
-      <c r="Z5" s="18"/>
-      <c r="AA5" s="18"/>
-      <c r="AB5" s="18"/>
-      <c r="AC5" s="18"/>
-      <c r="AD5" s="18"/>
-      <c r="AE5" s="18"/>
-      <c r="AF5" s="18"/>
-      <c r="AG5" s="18"/>
-      <c r="AH5" s="18"/>
+    <row r="5" spans="1:36" ht="13.5" customHeight="1" thickBot="1">
+      <c r="A5" s="26"/>
+      <c r="B5" s="26"/>
+      <c r="C5" s="26"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="26"/>
+      <c r="F5" s="26"/>
+      <c r="G5" s="26"/>
+      <c r="H5" s="26"/>
+      <c r="I5" s="26"/>
+      <c r="J5" s="26"/>
+      <c r="K5" s="26"/>
+      <c r="L5" s="26"/>
+      <c r="M5" s="26"/>
+      <c r="N5" s="26"/>
+      <c r="O5" s="26"/>
+      <c r="P5" s="26"/>
+      <c r="Q5" s="26"/>
+      <c r="R5" s="26"/>
+      <c r="S5" s="26"/>
+      <c r="T5" s="26"/>
+      <c r="U5" s="26"/>
+      <c r="V5" s="26"/>
+      <c r="W5" s="26"/>
+      <c r="X5" s="26"/>
+      <c r="Y5" s="26"/>
+      <c r="Z5" s="26"/>
+      <c r="AA5" s="26"/>
+      <c r="AB5" s="26"/>
+      <c r="AC5" s="26"/>
+      <c r="AD5" s="26"/>
+      <c r="AE5" s="26"/>
+      <c r="AF5" s="26"/>
+      <c r="AG5" s="26"/>
+      <c r="AH5" s="26"/>
       <c r="AI5" s="10"/>
       <c r="AJ5" s="10"/>
     </row>
-    <row r="6" spans="1:36">
+    <row r="6" spans="1:36" ht="13.5" customHeight="1">
       <c r="A6" s="11"/>
       <c r="B6" s="19"/>
       <c r="C6" s="20"/>
@@ -845,10 +847,10 @@
       <c r="AI6" s="21"/>
       <c r="AJ6" s="22"/>
     </row>
-    <row r="7" spans="1:36">
+    <row r="7" spans="1:36" ht="13.5" customHeight="1">
       <c r="A7" s="13"/>
-      <c r="B7" s="23"/>
-      <c r="C7" s="24"/>
+      <c r="B7" s="15"/>
+      <c r="C7" s="16"/>
       <c r="D7" s="14"/>
       <c r="E7" s="14"/>
       <c r="F7" s="14"/>
@@ -880,10 +882,10 @@
       <c r="AF7" s="14"/>
       <c r="AG7" s="14"/>
       <c r="AH7" s="14"/>
-      <c r="AI7" s="25"/>
-      <c r="AJ7" s="26"/>
-    </row>
-    <row r="8" spans="1:36">
+      <c r="AI7" s="17"/>
+      <c r="AJ7" s="18"/>
+    </row>
+    <row r="8" spans="1:36" ht="13.5" customHeight="1">
       <c r="A8" s="11"/>
       <c r="B8" s="19"/>
       <c r="C8" s="20"/>
@@ -921,10 +923,10 @@
       <c r="AI8" s="21"/>
       <c r="AJ8" s="22"/>
     </row>
-    <row r="9" spans="1:36">
+    <row r="9" spans="1:36" ht="13.5" customHeight="1">
       <c r="A9" s="13"/>
-      <c r="B9" s="23"/>
-      <c r="C9" s="24"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="16"/>
       <c r="D9" s="14"/>
       <c r="E9" s="14"/>
       <c r="F9" s="14"/>
@@ -956,10 +958,10 @@
       <c r="AF9" s="14"/>
       <c r="AG9" s="14"/>
       <c r="AH9" s="14"/>
-      <c r="AI9" s="25"/>
-      <c r="AJ9" s="26"/>
-    </row>
-    <row r="20" spans="1:19" s="1" customFormat="1">
+      <c r="AI9" s="17"/>
+      <c r="AJ9" s="18"/>
+    </row>
+    <row r="20" spans="1:19" s="1" customFormat="1" ht="13.5" customHeight="1">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -980,7 +982,7 @@
       <c r="R20" s="3"/>
       <c r="S20" s="3"/>
     </row>
-    <row r="21" spans="1:19" s="1" customFormat="1">
+    <row r="21" spans="1:19" s="1" customFormat="1" ht="13.5" customHeight="1">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -1001,7 +1003,7 @@
       <c r="R21" s="3"/>
       <c r="S21" s="3"/>
     </row>
-    <row r="22" spans="1:19" s="1" customFormat="1">
+    <row r="22" spans="1:19" s="1" customFormat="1" ht="13.5" customHeight="1">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -1024,21 +1026,21 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A2:C3"/>
+    <mergeCell ref="AI2:AJ3"/>
+    <mergeCell ref="A4:AH4"/>
+    <mergeCell ref="A5:AH5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="AI6:AJ6"/>
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="AI7:AJ7"/>
     <mergeCell ref="B8:C8"/>
     <mergeCell ref="AI8:AJ8"/>
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="AI9:AJ9"/>
-    <mergeCell ref="A2:C3"/>
-    <mergeCell ref="AI2:AJ3"/>
-    <mergeCell ref="A4:AH4"/>
-    <mergeCell ref="A5:AH5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="AI6:AJ6"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
-  <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.97916666666666663" bottom="0.39370078740157483" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.98425196850393704" bottom="0.39370078740157483" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;L&amp;"ＭＳ ゴシック,Regular"&amp;7勤次郎株式会社&amp;C&amp;"ＭＳ ゴシック,Regular"&amp;12振休確認表(日数管理_紐付あり_年月日)&amp;R&amp;"ＭＳ ゴシック,Regular"&amp;7&amp;D　&amp;T　

</xml_diff>